<commit_message>
Fix 5bus esd1 case
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_uced_esd1.xlsx
+++ b/ams/cases/5bus/pjm5bus_uced_esd1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE4C99C-7E87-5641-9352-3DA1DF57442A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944A19A0-37C0-D742-B090-BAF670D3ED03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="162">
   <si>
     <t>idx</t>
   </si>
@@ -449,9 +449,6 @@
   </si>
   <si>
     <t>ug</t>
-  </si>
-  <si>
-    <t>1,1,1,1</t>
   </si>
   <si>
     <r>
@@ -631,6 +628,30 @@
   </si>
   <si>
     <t>Line AB2</t>
+  </si>
+  <si>
+    <t>PV_2</t>
+  </si>
+  <si>
+    <t>PV 2</t>
+  </si>
+  <si>
+    <t>GCost_5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>SFRC_5</t>
+  </si>
+  <si>
+    <t>SRC_5</t>
+  </si>
+  <si>
+    <t>NSRC_5</t>
+  </si>
+  <si>
+    <t>1,1,1,1,1</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1280,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1295,7 +1316,7 @@
         <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">
@@ -1312,7 +1333,7 @@
         <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16">
@@ -1329,7 +1350,7 @@
         <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16">
@@ -1346,7 +1367,7 @@
         <v>112</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16">
@@ -1726,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369B7ED6-0339-A34F-8D4C-28B9C408DB19}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView zoomScale="207" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1819,7 +1840,25 @@
         <v>72</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1901,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB172BE7-B3C0-A449-8F62-0781AC3DED02}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD11"/>
+    <sheetView zoomScale="230" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1979,7 +2018,22 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2061,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF8DCDA-3E95-6745-801C-7005462F6D2D}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2139,7 +2193,22 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2559,11 +2628,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2821,7 +2890,70 @@
         <v>0.3</v>
       </c>
     </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>230</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>99</v>
+      </c>
+      <c r="L5">
+        <v>-99</v>
+      </c>
+      <c r="M5">
+        <v>99</v>
+      </c>
+      <c r="N5">
+        <v>-99</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1.4</v>
+      </c>
+      <c r="Q5">
+        <v>0.6</v>
+      </c>
+      <c r="R5">
+        <v>0.5</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0.01</v>
+      </c>
+      <c r="U5">
+        <v>0.3</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2830,51 +2962,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD37CC2-7295-9745-AE86-E7562082AFC8}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>145</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -2882,19 +3014,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="14">
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="G2" s="14">
         <v>100</v>
@@ -3078,10 +3210,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3261,7 +3393,43 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3270,9 +3438,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomLeft" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3371,7 +3539,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -3445,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3519,7 +3687,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3593,7 +3761,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3667,7 +3835,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -3741,7 +3909,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -3815,7 +3983,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8">
         <v>0</v>

</xml_diff>

<commit_message>
[WIP] Refactor test_dctypes, refactor test_rtn_rted
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_uced_esd1.xlsx
+++ b/ams/cases/5bus/pjm5bus_uced_esd1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/5bus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1A8D6E-CDFB-CC48-9536-4DDE21741093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0647B3F-81E1-4544-9333-03E5AC5A42B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -3350,8 +3350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3560,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -3576,7 +3576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
     </sheetView>

</xml_diff>